<commit_message>
testing on all test cases
</commit_message>
<xml_diff>
--- a/Output_Comparison.xlsx
+++ b/Output_Comparison.xlsx
@@ -531,7 +531,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>{'OR ART. 214 Abs. 1', 'OR ART. 184 Abs. 1', 'OR ART. 185 Abs. 1'}</t>
+          <t>{'OR ART. 185 Abs. 1', 'OR ART. 184 Abs. 1', 'OR ART. 214 Abs. 1'}</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -567,7 +567,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>{'OR ART. 185 Abs. 1', 'OR ART. 119 Abs. 1', 'OR ART. 119 Abs. 2', 'OR ART. 185 Abs. 2', 'OR ART. 119 Abs. 3'}</t>
+          <t>{'OR ART. 109 Abs. 1', 'OR ART. 119 Abs. 1', 'OR ART. 185 Abs. 1', 'OR ART. 185 Abs. 2', 'OR ART. 119 Abs. 3', 'OR ART. 119 Abs. 2'}</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -603,10 +603,18 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>{'OR ART. 259e', 'OR ART. 257g', 'OR ART. 259d', 'OR ART. 266g'}</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -679,10 +687,18 @@
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>{'StGB Art. 179quater', 'OR Art. 19 Abs. 1', 'UrhG Art. 11 Abs. 2', 'ZGB Art. 28a', 'UrhG Art. 13', 'OR Art. 67 Abs. 1', 'OR Art. 41', 'UrhG Art. 20', 'UrhG Art. 28', 'UrhG Art. 15', 'OR Art. 97 Abs. 1', 'OR Art. 423 Abs. 1', 'UrhG Art. 29', 'ZGB Art. 328b', 'UrhG Art. 19 Abs. 1', 'OR Art. 62 Abs. 1', 'UrhG Art. 40', 'ZGB Art. 28 Abs. 1', 'UrhG Art. 36', 'ZGB Art. 28 Abs. 2'}</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
@@ -723,10 +739,18 @@
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>{'OR ART. 18', 'OR ART. 24', 'OR ART. 23', 'OR ART. 97', 'OR ART. 367', 'OR ART. 404', 'OR ART. 364', 'OR ART. 107', 'OR ART. 1', 'OR ART. 363', 'OR ART. 109'}</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -764,10 +788,18 @@
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>{'OR ART. 330c', 'OR ART. 330b', 'OR ART. 330a', 'OR ART. 335'}</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -797,10 +829,18 @@
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>{'OR ART. 185 Abs. 1', 'OR ART. 184 Abs. 1', 'OR ART. 214 Abs. 1'}</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -836,10 +876,18 @@
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>{'OR ART. 109 Abs. 1', 'OR ART. 119 Abs. 1', 'OR ART. 185 Abs. 1', 'OR ART. 185 Abs. 2', 'OR ART. 119 Abs. 3', 'OR ART. 119 Abs. 2'}</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
@@ -875,10 +923,18 @@
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>{'OR ART. 185 Abs. 1', 'OR ART. 119 Abs. 1', 'OR ART. 109', 'OR ART. 119 Abs. 2'}</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -912,10 +968,18 @@
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>{'OR ART. 185 Abs. 1', 'OR ART. 185 Abs. 3', 'OR ART. 185 Abs. 2', 'OR ART. 99 Abs. 3'}</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>

</xml_diff>